<commit_message>
added columns for additional incentives on the employee list
</commit_message>
<xml_diff>
--- a/Payroll-Demo.xlsx
+++ b/Payroll-Demo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\slu teaching stuff\octoberfest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\THE PMO CO\Documents\GitHub\payroll_demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302B5C41-9761-4DAD-A240-27A9032B0307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D17F5F-0AD7-405A-A132-E25F47B6F9BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="770" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="770" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data1" sheetId="25" state="hidden" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="280">
   <si>
     <t>Status</t>
   </si>
@@ -1379,6 +1379,18 @@
   </si>
   <si>
     <t>whichever is lower</t>
+  </si>
+  <si>
+    <t>This is assignment</t>
+  </si>
+  <si>
+    <t>Holiday Pay</t>
+  </si>
+  <si>
+    <t>Overtime Pay</t>
+  </si>
+  <si>
+    <t>Night DifferentialPay</t>
   </si>
 </sst>
 </file>
@@ -2875,7 +2887,7 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="389">
+  <cellXfs count="390">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3730,18 +3742,6 @@
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="22" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="22" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3781,12 +3781,24 @@
     <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="43" fontId="22" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="43" fontId="22" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3856,6 +3868,39 @@
     <xf numFmtId="0" fontId="19" fillId="7" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="45" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3913,39 +3958,7 @@
     <xf numFmtId="0" fontId="17" fillId="38" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -6922,7 +6935,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" ht="14.4">
       <c r="A6" s="166">
         <v>3250</v>
       </c>
@@ -6978,7 +6991,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" ht="14.4">
       <c r="A7" s="166">
         <v>3750</v>
       </c>
@@ -7034,7 +7047,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" ht="14.4">
       <c r="A8" s="166">
         <v>4250</v>
       </c>
@@ -7090,7 +7103,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" ht="14.4">
       <c r="A9" s="166">
         <v>4750</v>
       </c>
@@ -7146,7 +7159,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" ht="14.4">
       <c r="A10" s="166">
         <v>5250</v>
       </c>
@@ -7202,7 +7215,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" ht="14.4">
       <c r="A11" s="166">
         <v>5750</v>
       </c>
@@ -7258,7 +7271,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" ht="14.4">
       <c r="A12" s="166">
         <v>6250</v>
       </c>
@@ -7314,7 +7327,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" ht="14.4">
       <c r="A13" s="166">
         <v>6750</v>
       </c>
@@ -7370,7 +7383,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" ht="14.4">
       <c r="A14" s="166">
         <v>7250</v>
       </c>
@@ -9424,32 +9437,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="359" t="s">
+      <c r="A1" s="370" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="359"/>
-      <c r="C1" s="359"/>
-      <c r="D1" s="359"/>
-      <c r="E1" s="359"/>
-      <c r="F1" s="359"/>
-      <c r="G1" s="359"/>
-      <c r="H1" s="359"/>
-      <c r="I1" s="359"/>
-      <c r="J1" s="359"/>
-      <c r="K1" s="359"/>
+      <c r="B1" s="370"/>
+      <c r="C1" s="370"/>
+      <c r="D1" s="370"/>
+      <c r="E1" s="370"/>
+      <c r="F1" s="370"/>
+      <c r="G1" s="370"/>
+      <c r="H1" s="370"/>
+      <c r="I1" s="370"/>
+      <c r="J1" s="370"/>
+      <c r="K1" s="370"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="359"/>
-      <c r="B2" s="359"/>
-      <c r="C2" s="359"/>
-      <c r="D2" s="359"/>
-      <c r="E2" s="359"/>
-      <c r="F2" s="359"/>
-      <c r="G2" s="359"/>
-      <c r="H2" s="359"/>
-      <c r="I2" s="359"/>
-      <c r="J2" s="359"/>
-      <c r="K2" s="359"/>
+      <c r="A2" s="370"/>
+      <c r="B2" s="370"/>
+      <c r="C2" s="370"/>
+      <c r="D2" s="370"/>
+      <c r="E2" s="370"/>
+      <c r="F2" s="370"/>
+      <c r="G2" s="370"/>
+      <c r="H2" s="370"/>
+      <c r="I2" s="370"/>
+      <c r="J2" s="370"/>
+      <c r="K2" s="370"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="185" t="s">
@@ -9755,24 +9768,24 @@
     </row>
     <row r="46" spans="1:8" ht="12.75" customHeight="1">
       <c r="A46" s="156"/>
-      <c r="B46" s="360" t="s">
+      <c r="B46" s="371" t="s">
         <v>174</v>
       </c>
-      <c r="C46" s="361"/>
-      <c r="D46" s="361"/>
-      <c r="E46" s="362"/>
+      <c r="C46" s="372"/>
+      <c r="D46" s="372"/>
+      <c r="E46" s="373"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="B47" s="363"/>
-      <c r="C47" s="364"/>
-      <c r="D47" s="364"/>
-      <c r="E47" s="365"/>
+      <c r="B47" s="374"/>
+      <c r="C47" s="375"/>
+      <c r="D47" s="375"/>
+      <c r="E47" s="376"/>
     </row>
     <row r="48" spans="1:8">
-      <c r="B48" s="366"/>
-      <c r="C48" s="367"/>
-      <c r="D48" s="367"/>
-      <c r="E48" s="368"/>
+      <c r="B48" s="377"/>
+      <c r="C48" s="378"/>
+      <c r="D48" s="378"/>
+      <c r="E48" s="379"/>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="185" t="s">
@@ -9928,54 +9941,54 @@
       <c r="B82" s="188"/>
     </row>
     <row r="83" spans="1:10">
-      <c r="B83" s="369" t="s">
+      <c r="B83" s="380" t="s">
         <v>203</v>
       </c>
-      <c r="C83" s="369"/>
-      <c r="D83" s="369"/>
-      <c r="E83" s="369"/>
-      <c r="F83" s="369"/>
-      <c r="G83" s="369"/>
-      <c r="H83" s="369"/>
-      <c r="I83" s="369"/>
-      <c r="J83" s="369"/>
+      <c r="C83" s="380"/>
+      <c r="D83" s="380"/>
+      <c r="E83" s="380"/>
+      <c r="F83" s="380"/>
+      <c r="G83" s="380"/>
+      <c r="H83" s="380"/>
+      <c r="I83" s="380"/>
+      <c r="J83" s="380"/>
     </row>
     <row r="84" spans="1:10">
-      <c r="B84" s="369"/>
-      <c r="C84" s="369"/>
-      <c r="D84" s="369"/>
-      <c r="E84" s="369"/>
-      <c r="F84" s="369"/>
-      <c r="G84" s="369"/>
-      <c r="H84" s="369"/>
-      <c r="I84" s="369"/>
-      <c r="J84" s="369"/>
+      <c r="B84" s="380"/>
+      <c r="C84" s="380"/>
+      <c r="D84" s="380"/>
+      <c r="E84" s="380"/>
+      <c r="F84" s="380"/>
+      <c r="G84" s="380"/>
+      <c r="H84" s="380"/>
+      <c r="I84" s="380"/>
+      <c r="J84" s="380"/>
     </row>
     <row r="85" spans="1:10">
-      <c r="A85" s="370" t="s">
+      <c r="A85" s="381" t="s">
         <v>204</v>
       </c>
       <c r="B85" s="209"/>
       <c r="C85" s="209"/>
-      <c r="E85" s="374" t="s">
+      <c r="E85" s="385" t="s">
         <v>205</v>
       </c>
-      <c r="F85" s="374"/>
-      <c r="G85" s="374"/>
-      <c r="H85" s="375"/>
+      <c r="F85" s="385"/>
+      <c r="G85" s="385"/>
+      <c r="H85" s="386"/>
     </row>
     <row r="86" spans="1:10">
-      <c r="A86" s="371"/>
+      <c r="A86" s="382"/>
       <c r="B86" s="198" t="s">
         <v>206</v>
       </c>
       <c r="C86" s="198" t="s">
         <v>207</v>
       </c>
-      <c r="E86" s="376"/>
-      <c r="F86" s="376"/>
-      <c r="G86" s="376"/>
-      <c r="H86" s="377"/>
+      <c r="E86" s="387"/>
+      <c r="F86" s="387"/>
+      <c r="G86" s="387"/>
+      <c r="H86" s="388"/>
     </row>
     <row r="87" spans="1:10">
       <c r="A87" s="210" t="s">
@@ -9988,11 +10001,11 @@
         <f>VLOOKUP(B87,$E$88:$H$92,4,1)</f>
         <v>EE</v>
       </c>
-      <c r="E87" s="384" t="s">
+      <c r="E87" s="365" t="s">
         <v>206</v>
       </c>
-      <c r="F87" s="384"/>
-      <c r="G87" s="384"/>
+      <c r="F87" s="365"/>
+      <c r="G87" s="365"/>
       <c r="H87" s="249" t="s">
         <v>209</v>
       </c>
@@ -10111,26 +10124,26 @@
       </c>
     </row>
     <row r="93" spans="1:10">
-      <c r="A93" s="372" t="s">
+      <c r="A93" s="383" t="s">
         <v>218</v>
       </c>
       <c r="B93" s="212"/>
       <c r="C93" s="212"/>
     </row>
     <row r="94" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A94" s="371"/>
+      <c r="A94" s="382"/>
       <c r="B94" s="213" t="s">
         <v>219</v>
       </c>
       <c r="C94" s="214" t="s">
         <v>207</v>
       </c>
-      <c r="F94" s="373" t="s">
+      <c r="F94" s="384" t="s">
         <v>220</v>
       </c>
-      <c r="G94" s="373"/>
-      <c r="H94" s="373"/>
-      <c r="I94" s="373"/>
+      <c r="G94" s="384"/>
+      <c r="H94" s="384"/>
+      <c r="I94" s="384"/>
     </row>
     <row r="95" spans="1:10">
       <c r="A95" s="215" t="s">
@@ -10138,18 +10151,18 @@
       </c>
       <c r="B95" s="212"/>
       <c r="C95" s="200"/>
-      <c r="F95" s="373"/>
-      <c r="G95" s="373"/>
-      <c r="H95" s="373"/>
-      <c r="I95" s="373"/>
+      <c r="F95" s="384"/>
+      <c r="G95" s="384"/>
+      <c r="H95" s="384"/>
+      <c r="I95" s="384"/>
     </row>
     <row r="96" spans="1:10">
       <c r="A96" s="216"/>
       <c r="B96" s="187"/>
-      <c r="F96" s="373"/>
-      <c r="G96" s="373"/>
-      <c r="H96" s="373"/>
-      <c r="I96" s="373"/>
+      <c r="F96" s="384"/>
+      <c r="G96" s="384"/>
+      <c r="H96" s="384"/>
+      <c r="I96" s="384"/>
     </row>
     <row r="98" spans="1:9">
       <c r="A98" s="185" t="s">
@@ -10190,11 +10203,11 @@
       <c r="A106" s="187" t="s">
         <v>229</v>
       </c>
-      <c r="G106" s="388" t="s">
+      <c r="G106" s="369" t="s">
         <v>230</v>
       </c>
-      <c r="H106" s="388"/>
-      <c r="I106" s="388"/>
+      <c r="H106" s="369"/>
+      <c r="I106" s="369"/>
     </row>
     <row r="107" spans="1:9">
       <c r="B107" s="193" t="s">
@@ -10209,34 +10222,34 @@
       <c r="E107" s="193" t="s">
         <v>233</v>
       </c>
-      <c r="G107" s="388"/>
-      <c r="H107" s="388"/>
-      <c r="I107" s="388"/>
+      <c r="G107" s="369"/>
+      <c r="H107" s="369"/>
+      <c r="I107" s="369"/>
     </row>
     <row r="108" spans="1:9">
       <c r="A108" s="193" t="str">
         <f t="array" ref="A108:A111">TRANSPOSE(B107:E107)</f>
         <v>Name</v>
       </c>
-      <c r="G108" s="388"/>
-      <c r="H108" s="388"/>
-      <c r="I108" s="388"/>
+      <c r="G108" s="369"/>
+      <c r="H108" s="369"/>
+      <c r="I108" s="369"/>
     </row>
     <row r="109" spans="1:9">
       <c r="A109" s="193" t="str">
         <v>Gender</v>
       </c>
-      <c r="G109" s="388"/>
-      <c r="H109" s="388"/>
-      <c r="I109" s="388"/>
+      <c r="G109" s="369"/>
+      <c r="H109" s="369"/>
+      <c r="I109" s="369"/>
     </row>
     <row r="110" spans="1:9">
       <c r="A110" s="193" t="str">
         <v>Age</v>
       </c>
-      <c r="G110" s="388"/>
-      <c r="H110" s="388"/>
-      <c r="I110" s="388"/>
+      <c r="G110" s="369"/>
+      <c r="H110" s="369"/>
+      <c r="I110" s="369"/>
     </row>
     <row r="111" spans="1:9">
       <c r="A111" s="193" t="str">
@@ -10248,17 +10261,17 @@
     </row>
     <row r="116" spans="1:11" ht="13.8" thickBot="1"/>
     <row r="117" spans="1:11" ht="21" thickBot="1">
-      <c r="A117" s="378" t="s">
+      <c r="A117" s="359" t="s">
         <v>237</v>
       </c>
-      <c r="B117" s="379"/>
-      <c r="C117" s="379"/>
-      <c r="D117" s="379"/>
-      <c r="E117" s="379"/>
-      <c r="F117" s="379"/>
-      <c r="G117" s="379"/>
-      <c r="H117" s="379"/>
-      <c r="I117" s="380"/>
+      <c r="B117" s="360"/>
+      <c r="C117" s="360"/>
+      <c r="D117" s="360"/>
+      <c r="E117" s="360"/>
+      <c r="F117" s="360"/>
+      <c r="G117" s="360"/>
+      <c r="H117" s="360"/>
+      <c r="I117" s="361"/>
     </row>
     <row r="118" spans="1:11" ht="15">
       <c r="A118" s="217" t="s">
@@ -10307,12 +10320,12 @@
       <c r="E123" s="221">
         <v>54</v>
       </c>
-      <c r="H123" s="385" t="s">
+      <c r="H123" s="366" t="s">
         <v>242</v>
       </c>
-      <c r="I123" s="386"/>
-      <c r="J123" s="386"/>
-      <c r="K123" s="387"/>
+      <c r="I123" s="367"/>
+      <c r="J123" s="367"/>
+      <c r="K123" s="368"/>
     </row>
     <row r="124" spans="1:11" s="217" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A124" s="222" t="s">
@@ -10371,12 +10384,12 @@
       <c r="E126" s="223">
         <v>29</v>
       </c>
-      <c r="H126" s="385" t="s">
+      <c r="H126" s="366" t="s">
         <v>266</v>
       </c>
-      <c r="I126" s="386"/>
-      <c r="J126" s="386"/>
-      <c r="K126" s="387"/>
+      <c r="I126" s="367"/>
+      <c r="J126" s="367"/>
+      <c r="K126" s="368"/>
     </row>
     <row r="127" spans="1:11" s="217" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A127" s="225" t="s">
@@ -10404,17 +10417,17 @@
     </row>
     <row r="128" spans="1:11" s="217" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1"/>
     <row r="129" spans="1:18" ht="21" thickBot="1">
-      <c r="A129" s="378" t="s">
+      <c r="A129" s="359" t="s">
         <v>244</v>
       </c>
-      <c r="B129" s="379"/>
-      <c r="C129" s="379"/>
-      <c r="D129" s="379"/>
-      <c r="E129" s="379"/>
-      <c r="F129" s="379"/>
-      <c r="G129" s="379"/>
-      <c r="H129" s="379"/>
-      <c r="I129" s="380"/>
+      <c r="B129" s="360"/>
+      <c r="C129" s="360"/>
+      <c r="D129" s="360"/>
+      <c r="E129" s="360"/>
+      <c r="F129" s="360"/>
+      <c r="G129" s="360"/>
+      <c r="H129" s="360"/>
+      <c r="I129" s="361"/>
     </row>
     <row r="130" spans="1:18" ht="15">
       <c r="A130" s="217" t="s">
@@ -10573,17 +10586,17 @@
     <row r="140" spans="1:18" ht="20.100000000000001" customHeight="1"/>
     <row r="141" spans="1:18" ht="20.100000000000001" customHeight="1" thickBot="1"/>
     <row r="142" spans="1:18" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A142" s="378" t="s">
+      <c r="A142" s="359" t="s">
         <v>247</v>
       </c>
-      <c r="B142" s="379"/>
-      <c r="C142" s="379"/>
-      <c r="D142" s="379"/>
-      <c r="E142" s="379"/>
-      <c r="F142" s="379"/>
-      <c r="G142" s="379"/>
-      <c r="H142" s="379"/>
-      <c r="I142" s="380"/>
+      <c r="B142" s="360"/>
+      <c r="C142" s="360"/>
+      <c r="D142" s="360"/>
+      <c r="E142" s="360"/>
+      <c r="F142" s="360"/>
+      <c r="G142" s="360"/>
+      <c r="H142" s="360"/>
+      <c r="I142" s="361"/>
     </row>
     <row r="143" spans="1:18" ht="20.100000000000001" customHeight="1" thickBot="1"/>
     <row r="144" spans="1:18" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -10700,12 +10713,12 @@
       <c r="D155" s="217"/>
     </row>
     <row r="156" spans="1:6" ht="30" customHeight="1" thickBot="1">
-      <c r="A156" s="381" t="s">
+      <c r="A156" s="362" t="s">
         <v>252</v>
       </c>
-      <c r="B156" s="382"/>
-      <c r="C156" s="382"/>
-      <c r="D156" s="383"/>
+      <c r="B156" s="363"/>
+      <c r="C156" s="363"/>
+      <c r="D156" s="364"/>
     </row>
     <row r="157" spans="1:6" ht="30" customHeight="1" thickBot="1">
       <c r="A157" s="240" t="s">
@@ -10765,6 +10778,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:K2"/>
+    <mergeCell ref="B46:E48"/>
+    <mergeCell ref="B83:J84"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="F94:I96"/>
+    <mergeCell ref="E85:H86"/>
     <mergeCell ref="A129:I129"/>
     <mergeCell ref="A142:I142"/>
     <mergeCell ref="A156:D156"/>
@@ -10773,13 +10793,6 @@
     <mergeCell ref="H123:K123"/>
     <mergeCell ref="H126:K126"/>
     <mergeCell ref="G106:I110"/>
-    <mergeCell ref="A1:K2"/>
-    <mergeCell ref="B46:E48"/>
-    <mergeCell ref="B83:J84"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="F94:I96"/>
-    <mergeCell ref="E85:H86"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B144" xr:uid="{D82B5E39-5E8B-4915-9E95-0DCEB35A848F}">
@@ -13510,10 +13523,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ED3AAC6-301D-4C15-B573-3AF8384821ED}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView zoomScale="166" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:F14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="166" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
@@ -13524,10 +13537,13 @@
     <col min="4" max="4" width="16.33203125" style="122" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5546875" style="122" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5546875" style="122" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="122"/>
+    <col min="7" max="7" width="8.88671875" style="122"/>
+    <col min="8" max="8" width="16.33203125" style="122" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" style="122" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="122"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:11">
       <c r="A1" s="315" t="s">
         <v>274</v>
       </c>
@@ -13536,8 +13552,11 @@
       <c r="D1" s="316"/>
       <c r="E1" s="316"/>
       <c r="F1" s="316"/>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="H1" s="122" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="123" t="s">
         <v>119</v>
       </c>
@@ -13556,8 +13575,18 @@
       <c r="F2" s="123" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="H2" s="389" t="s">
+        <v>277</v>
+      </c>
+      <c r="I2" s="389" t="s">
+        <v>278</v>
+      </c>
+      <c r="J2" s="389" t="s">
+        <v>279</v>
+      </c>
+      <c r="K2" s="389"/>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="152">
         <v>1</v>
       </c>
@@ -13576,8 +13605,12 @@
       <c r="F3" s="138">
         <v>85</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="H3" s="389"/>
+      <c r="I3" s="389"/>
+      <c r="J3" s="389"/>
+      <c r="K3" s="389"/>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="152">
         <v>2</v>
       </c>
@@ -13596,8 +13629,12 @@
       <c r="F4" s="138">
         <v>85</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="H4" s="389"/>
+      <c r="I4" s="389"/>
+      <c r="J4" s="389"/>
+      <c r="K4" s="389"/>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="152">
         <v>3</v>
       </c>
@@ -13616,8 +13653,12 @@
       <c r="F5" s="138">
         <v>85</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="H5" s="389"/>
+      <c r="I5" s="389"/>
+      <c r="J5" s="389"/>
+      <c r="K5" s="389"/>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="152">
         <v>4</v>
       </c>
@@ -13634,8 +13675,12 @@
       <c r="F6" s="138">
         <v>85</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="H6" s="389"/>
+      <c r="I6" s="389"/>
+      <c r="J6" s="389"/>
+      <c r="K6" s="389"/>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="152">
         <v>5</v>
       </c>
@@ -13654,6 +13699,10 @@
       <c r="F7" s="138">
         <v>85</v>
       </c>
+      <c r="H7" s="389"/>
+      <c r="I7" s="389"/>
+      <c r="J7" s="389"/>
+      <c r="K7" s="389"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -13667,7 +13716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9E99DB6-97E5-4E70-B037-4901957D7550}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:D2"/>
     </sheetView>
   </sheetViews>
@@ -13680,24 +13729,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.2" customHeight="1">
-      <c r="A1" s="323" t="s">
+      <c r="A1" s="319" t="s">
         <v>131</v>
       </c>
-      <c r="B1" s="324"/>
-      <c r="C1" s="324"/>
-      <c r="D1" s="324"/>
-      <c r="E1" s="324"/>
-      <c r="F1" s="325"/>
+      <c r="B1" s="320"/>
+      <c r="C1" s="320"/>
+      <c r="D1" s="320"/>
+      <c r="E1" s="320"/>
+      <c r="F1" s="321"/>
     </row>
     <row r="2" spans="1:9" ht="25.2" customHeight="1">
       <c r="A2" s="151" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="326">
+      <c r="B2" s="322">
         <v>1</v>
       </c>
-      <c r="C2" s="326"/>
-      <c r="D2" s="326"/>
+      <c r="C2" s="322"/>
+      <c r="D2" s="322"/>
       <c r="E2" s="121"/>
       <c r="F2" s="145"/>
     </row>
@@ -13705,12 +13754,12 @@
       <c r="A3" s="151" t="s">
         <v>120</v>
       </c>
-      <c r="B3" s="327" t="str">
+      <c r="B3" s="323" t="str">
         <f>VLOOKUP(B2,'Payroll Data'!A2:E7,2,0)</f>
         <v>Jayden Johnson</v>
       </c>
-      <c r="C3" s="327"/>
-      <c r="D3" s="327"/>
+      <c r="C3" s="323"/>
+      <c r="D3" s="323"/>
       <c r="E3" s="121"/>
       <c r="F3" s="145"/>
     </row>
@@ -13718,12 +13767,12 @@
       <c r="A4" s="151" t="s">
         <v>121</v>
       </c>
-      <c r="B4" s="328" t="str">
+      <c r="B4" s="324" t="str">
         <f>VLOOKUP(B2,'Payroll Data'!A2:E7,3,0)</f>
         <v>Sales Personnel</v>
       </c>
-      <c r="C4" s="328"/>
-      <c r="D4" s="328"/>
+      <c r="C4" s="324"/>
+      <c r="D4" s="324"/>
       <c r="E4" s="121"/>
       <c r="F4" s="145"/>
     </row>
@@ -13735,69 +13784,69 @@
       <c r="A6" s="147" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="320"/>
-      <c r="C6" s="320"/>
-      <c r="D6" s="317">
+      <c r="B6" s="330"/>
+      <c r="C6" s="330"/>
+      <c r="D6" s="331">
         <f>VLOOKUP(B2,'Payroll Data'!A2:E7,4,0)</f>
         <v>30000</v>
       </c>
-      <c r="E6" s="317"/>
+      <c r="E6" s="331"/>
       <c r="F6" s="145"/>
     </row>
     <row r="7" spans="1:9" ht="25.2" customHeight="1">
       <c r="A7" s="147" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="320"/>
-      <c r="C7" s="320"/>
-      <c r="D7" s="317">
+      <c r="B7" s="330"/>
+      <c r="C7" s="330"/>
+      <c r="D7" s="331">
         <f>VLOOKUP(B2,'Payroll Data'!A2:E7,5,0)</f>
         <v>5500</v>
       </c>
-      <c r="E7" s="317"/>
+      <c r="E7" s="331"/>
       <c r="F7" s="145"/>
     </row>
     <row r="8" spans="1:9" ht="25.2" customHeight="1">
       <c r="A8" s="147" t="s">
         <v>97</v>
       </c>
-      <c r="B8" s="320"/>
-      <c r="C8" s="320"/>
-      <c r="D8" s="318">
+      <c r="B8" s="330"/>
+      <c r="C8" s="330"/>
+      <c r="D8" s="334">
         <f>D6+D7</f>
         <v>35500</v>
       </c>
-      <c r="E8" s="319"/>
+      <c r="E8" s="335"/>
       <c r="F8" s="145"/>
     </row>
     <row r="9" spans="1:9" ht="25.2" customHeight="1">
-      <c r="A9" s="329" t="s">
+      <c r="A9" s="325" t="s">
         <v>98</v>
       </c>
-      <c r="B9" s="330"/>
-      <c r="C9" s="330"/>
+      <c r="B9" s="326"/>
+      <c r="C9" s="326"/>
       <c r="F9" s="145"/>
     </row>
     <row r="10" spans="1:9" ht="25.2" customHeight="1">
       <c r="A10" s="147" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="317">
+      <c r="B10" s="331">
         <f>VLOOKUP(D8,SSS!A5:R49,17,1)</f>
         <v>1125</v>
       </c>
-      <c r="C10" s="317"/>
+      <c r="C10" s="331"/>
       <c r="F10" s="145"/>
     </row>
     <row r="11" spans="1:9" ht="25.2" customHeight="1">
       <c r="A11" s="147" t="s">
         <v>99</v>
       </c>
-      <c r="B11" s="317">
+      <c r="B11" s="331">
         <f>IF(D8&lt;=10000,400,IF(D8&lt;=80000,D8*0.04,3200))</f>
         <v>1420</v>
       </c>
-      <c r="C11" s="317"/>
+      <c r="C11" s="331"/>
       <c r="D11" s="154"/>
       <c r="F11" s="145"/>
     </row>
@@ -13805,11 +13854,11 @@
       <c r="A12" s="147" t="s">
         <v>100</v>
       </c>
-      <c r="B12" s="331">
+      <c r="B12" s="327">
         <f>IF(D8&gt;=5000,100,IF(D8&gt;=1500,D8*0.02,D8*0.01))</f>
         <v>100</v>
       </c>
-      <c r="C12" s="331"/>
+      <c r="C12" s="327"/>
       <c r="D12" s="144" t="s">
         <v>275</v>
       </c>
@@ -13819,32 +13868,32 @@
       <c r="A13" s="147"/>
       <c r="B13" s="121"/>
       <c r="C13" s="121"/>
-      <c r="D13" s="317">
+      <c r="D13" s="331">
         <f>SUM(B10:C12)</f>
         <v>2645</v>
       </c>
-      <c r="E13" s="317"/>
+      <c r="E13" s="331"/>
       <c r="F13" s="145"/>
     </row>
     <row r="14" spans="1:9" ht="25.2" customHeight="1">
-      <c r="A14" s="332" t="s">
+      <c r="A14" s="328" t="s">
         <v>101</v>
       </c>
-      <c r="B14" s="333"/>
-      <c r="C14" s="333"/>
+      <c r="B14" s="329"/>
+      <c r="C14" s="329"/>
       <c r="F14" s="145"/>
     </row>
     <row r="15" spans="1:9" ht="25.2" customHeight="1">
       <c r="A15" s="147" t="s">
         <v>102</v>
       </c>
-      <c r="B15" s="335"/>
-      <c r="C15" s="335"/>
-      <c r="D15" s="317">
+      <c r="B15" s="333"/>
+      <c r="C15" s="333"/>
+      <c r="D15" s="331">
         <f>VLOOKUP(B2,'Payroll Data'!A2:F7,6,0)</f>
         <v>85</v>
       </c>
-      <c r="E15" s="317"/>
+      <c r="E15" s="331"/>
       <c r="F15" s="145"/>
       <c r="H15" s="154">
         <f>D16</f>
@@ -13855,11 +13904,11 @@
       <c r="A16" s="147" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="334">
+      <c r="D16" s="332">
         <f>D8-D13</f>
         <v>32855</v>
       </c>
-      <c r="E16" s="322"/>
+      <c r="E16" s="318"/>
       <c r="F16" s="145"/>
       <c r="G16" s="116">
         <f>HLOOKUP(D16,'Tax Table (Monthly)'!B3:G8,4,1)</f>
@@ -13878,11 +13927,11 @@
       <c r="A17" s="147" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="321">
+      <c r="D17" s="317">
         <f>HLOOKUP(D16,'Tax Table (Monthly)'!B3:G8,4,1)+(VALUE(LEFT(HLOOKUP(D16,'Tax Table (Monthly)'!B3:G8,6,1),3)*(D16-HLOOKUP(D16,'Tax Table (Monthly)'!B3:G8,1,1))))</f>
         <v>2404.4</v>
       </c>
-      <c r="E17" s="322"/>
+      <c r="E17" s="318"/>
       <c r="F17" s="145"/>
       <c r="G17" s="116">
         <f>(VALUE(LEFT(HLOOKUP(D16,'Tax Table (Monthly)'!B3:G8,6,1),3)*(D16-HLOOKUP(D16,'Tax Table (Monthly)'!B3:G8,1,1))))</f>
@@ -13897,11 +13946,11 @@
       <c r="A18" s="147" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="321">
+      <c r="D18" s="317">
         <f>D8-D13-D15-D17</f>
         <v>30365.599999999999</v>
       </c>
-      <c r="E18" s="322"/>
+      <c r="E18" s="318"/>
       <c r="F18" s="145"/>
     </row>
     <row r="19" spans="1:8">
@@ -13921,6 +13970,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="B7:C7"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="A1:F1"/>
@@ -13937,11 +13991,6 @@
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>